<commit_message>
updated member excel sheet
</commit_message>
<xml_diff>
--- a/MemberUpload.xlsx
+++ b/MemberUpload.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_640AEC97D912A7E17A53A47B27AE80612AA8EE96" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E38DE08-B974-4CEC-92CA-62AAD21DCB22}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACEAF89-5B37-4307-BDD9-086671692667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Ashwin</t>
+  </si>
+  <si>
+    <t>MbrNo</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,7 +423,7 @@
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -454,8 +457,11 @@
       <c r="K1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -489,8 +495,11 @@
       <c r="K2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -524,8 +533,11 @@
       <c r="K3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -559,8 +571,11 @@
       <c r="K4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -594,8 +609,11 @@
       <c r="K5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -629,8 +647,11 @@
       <c r="K6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -664,8 +685,11 @@
       <c r="K7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -699,8 +723,11 @@
       <c r="K8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -734,8 +761,11 @@
       <c r="K9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -769,8 +799,11 @@
       <c r="K10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -803,6 +836,9 @@
       </c>
       <c r="K11" t="s">
         <v>17</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added updated gi exe
</commit_message>
<xml_diff>
--- a/MemberUpload.xlsx
+++ b/MemberUpload.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACEAF89-5B37-4307-BDD9-086671692667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1953BB74-2C7A-4F99-95C0-0AE5BF390A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>CompanyID</t>
   </si>
   <si>
-    <t>GTL1</t>
-  </si>
-  <si>
     <t>AddressID</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>MbrNo</t>
+  </si>
+  <si>
+    <t>EEGP</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="K2" sqref="K2:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,10 +428,10 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -458,7 +458,7 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -493,7 +493,7 @@
         <v>75000</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -507,7 +507,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -531,7 +531,7 @@
         <v>120000</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -569,7 +569,7 @@
         <v>67000</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -607,7 +607,7 @@
         <v>75000</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -645,7 +645,7 @@
         <v>50000</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L6">
         <v>5</v>
@@ -659,10 +659,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
       </c>
       <c r="E7">
         <v>19951202</v>
@@ -683,7 +683,7 @@
         <v>89000</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L7">
         <v>6</v>
@@ -697,10 +697,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>19800101</v>
@@ -721,7 +721,7 @@
         <v>100000</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L8">
         <v>7</v>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -759,7 +759,7 @@
         <v>73000</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L9">
         <v>8</v>
@@ -773,10 +773,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <v>19930103</v>
@@ -797,7 +797,7 @@
         <v>75000</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L10">
         <v>9</v>
@@ -811,10 +811,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>19980104</v>
@@ -835,7 +835,7 @@
         <v>49000</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L11">
         <v>10</v>

</xml_diff>